<commit_message>
Stable version multiple sheets
</commit_message>
<xml_diff>
--- a/new.xlsx
+++ b/new.xlsx
@@ -37,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -63,13 +63,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
@@ -453,7 +446,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BR4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,81 +466,18 @@
         </is>
       </c>
       <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="n"/>
-      <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="n"/>
-      <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="n"/>
-      <c r="I1" s="1" t="n"/>
-      <c r="J1" s="1" t="n"/>
-      <c r="K1" s="1" t="n"/>
-      <c r="L1" s="1" t="n"/>
-      <c r="M1" s="1" t="n"/>
-      <c r="N1" s="1" t="n"/>
-      <c r="O1" s="1" t="n"/>
-      <c r="P1" s="1" t="n"/>
-      <c r="Q1" s="1" t="n"/>
-      <c r="R1" s="1" t="n"/>
-      <c r="S1" s="1" t="n"/>
-      <c r="T1" s="1" t="n"/>
-      <c r="U1" s="1" t="n"/>
-      <c r="V1" s="1" t="n"/>
-      <c r="W1" s="1" t="n"/>
-      <c r="X1" s="1" t="n"/>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>b</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="n"/>
-      <c r="AA1" s="1" t="n"/>
-      <c r="AB1" s="1" t="n"/>
-      <c r="AC1" s="1" t="n"/>
-      <c r="AD1" s="1" t="n"/>
-      <c r="AE1" s="1" t="n"/>
-      <c r="AF1" s="1" t="n"/>
-      <c r="AG1" s="1" t="n"/>
-      <c r="AH1" s="1" t="n"/>
-      <c r="AI1" s="1" t="n"/>
-      <c r="AJ1" s="1" t="n"/>
-      <c r="AK1" s="1" t="n"/>
-      <c r="AL1" s="1" t="n"/>
-      <c r="AM1" s="1" t="n"/>
-      <c r="AN1" s="1" t="n"/>
-      <c r="AO1" s="1" t="n"/>
-      <c r="AP1" s="1" t="n"/>
-      <c r="AQ1" s="1" t="n"/>
-      <c r="AR1" s="1" t="n"/>
-      <c r="AS1" s="1" t="n"/>
-      <c r="AT1" s="1" t="n"/>
-      <c r="AU1" s="1" t="n"/>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>c</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="n"/>
-      <c r="AX1" s="1" t="n"/>
-      <c r="AY1" s="1" t="n"/>
-      <c r="AZ1" s="1" t="n"/>
-      <c r="BA1" s="1" t="n"/>
-      <c r="BB1" s="1" t="n"/>
-      <c r="BC1" s="1" t="n"/>
-      <c r="BD1" s="1" t="n"/>
-      <c r="BE1" s="1" t="n"/>
-      <c r="BF1" s="1" t="n"/>
-      <c r="BG1" s="1" t="n"/>
-      <c r="BH1" s="1" t="n"/>
-      <c r="BI1" s="1" t="n"/>
-      <c r="BJ1" s="1" t="n"/>
-      <c r="BK1" s="1" t="n"/>
-      <c r="BL1" s="1" t="n"/>
-      <c r="BM1" s="1" t="n"/>
-      <c r="BN1" s="1" t="n"/>
-      <c r="BO1" s="1" t="n"/>
-      <c r="BP1" s="1" t="n"/>
-      <c r="BQ1" s="1" t="n"/>
-      <c r="BR1" s="1" t="n"/>
+      <c r="G1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -562,205 +492,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="J2" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="K2" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="M2" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="N2" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="O2" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="P2" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="R2" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="S2" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="T2" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="U2" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="V2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="W2" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="X2" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="Y2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="1" t="n">
         <v>1</v>
-      </c>
-      <c r="AA2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="AB2" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="AD2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="AE2" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="AF2" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="AG2" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="AH2" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="AI2" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="AJ2" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="AK2" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="AL2" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="AM2" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="AN2" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="AO2" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="AP2" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="AQ2" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="AR2" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="AS2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="AT2" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="AU2" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="AV2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="AY2" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="AZ2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="BA2" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="BB2" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="BC2" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="BD2" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="BE2" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="BF2" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="BG2" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="BH2" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="BI2" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="BJ2" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="BK2" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="BL2" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="BM2" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="BN2" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="BO2" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="BP2" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="BQ2" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="BR2" s="1" t="n">
-        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -775,108 +516,17 @@
         <v>5</v>
       </c>
       <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>7.0</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>7.0</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr"/>
-      <c r="AC4" t="inlineStr"/>
-      <c r="AD4" t="inlineStr"/>
-      <c r="AE4" t="inlineStr"/>
-      <c r="AF4" t="inlineStr"/>
-      <c r="AG4" t="inlineStr"/>
-      <c r="AH4" t="inlineStr"/>
-      <c r="AI4" t="inlineStr"/>
-      <c r="AJ4" t="inlineStr"/>
-      <c r="AK4" t="inlineStr"/>
-      <c r="AL4" t="inlineStr"/>
-      <c r="AM4" t="inlineStr"/>
-      <c r="AN4" t="inlineStr"/>
-      <c r="AO4" t="inlineStr"/>
-      <c r="AP4" t="inlineStr"/>
-      <c r="AQ4" t="inlineStr"/>
-      <c r="AR4" t="inlineStr"/>
-      <c r="AS4" t="inlineStr"/>
-      <c r="AT4" t="inlineStr"/>
-      <c r="AU4" t="inlineStr"/>
-      <c r="AV4" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
-      </c>
-      <c r="AW4" t="inlineStr">
-        <is>
-          <t>8.0</t>
-        </is>
-      </c>
-      <c r="AX4" t="inlineStr"/>
-      <c r="AY4" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="AZ4" t="inlineStr"/>
-      <c r="BA4" t="inlineStr"/>
-      <c r="BB4" t="inlineStr"/>
-      <c r="BC4" t="inlineStr"/>
-      <c r="BD4" t="inlineStr"/>
-      <c r="BE4" t="inlineStr"/>
-      <c r="BF4" t="inlineStr"/>
-      <c r="BG4" t="inlineStr"/>
-      <c r="BH4" t="inlineStr"/>
-      <c r="BI4" t="inlineStr"/>
-      <c r="BJ4" t="inlineStr"/>
-      <c r="BK4" t="inlineStr"/>
-      <c r="BL4" t="inlineStr"/>
-      <c r="BM4" t="inlineStr"/>
-      <c r="BN4" t="inlineStr"/>
-      <c r="BO4" t="inlineStr"/>
-      <c r="BP4" t="inlineStr"/>
-      <c r="BQ4" t="inlineStr"/>
-      <c r="BR4" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:X1"/>
-    <mergeCell ref="Y1:AU1"/>
-    <mergeCell ref="AV1:BR1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>